<commit_message>
db tool excel style via template
</commit_message>
<xml_diff>
--- a/DbTool/Template/StyleTemplate.xlsx
+++ b/DbTool/Template/StyleTemplate.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\AmandaChou\git\github\DevTool\DbTool\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAEBB31-3FAD-4952-9871-295ED3F62382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F88563-227F-4FF0-99A1-7A144641B7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37335" yWindow="3240" windowWidth="16095" windowHeight="9735" activeTab="1" xr2:uid="{93EE71A6-18E9-487D-ACF7-7CE2E333B3E7}"/>
+    <workbookView xWindow="6252" yWindow="888" windowWidth="16236" windowHeight="9696" xr2:uid="{93EE71A6-18E9-487D-ACF7-7CE2E333B3E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="StyleTemplate" sheetId="1" r:id="rId1"/>
-    <sheet name="StyleTemplate1" sheetId="4" r:id="rId2"/>
+    <sheet name="StyleTemplate" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,11 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>TableList 表頭樣式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>TableName 在各 sheet 樣式</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,100 +140,7 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -547,57 +449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EAFCD2-4FEB-4FF3-9738-83B38C37F97B}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73953184-80B9-45BC-A4A3-76DD0CE18A1C}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -607,27 +463,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>